<commit_message>
modificacion punto venta 21-09-2023
</commit_message>
<xml_diff>
--- a/COVENTAF/bin/Debug/Auto_Recuperacion_Factura.xlsx
+++ b/COVENTAF/bin/Debug/Auto_Recuperacion_Factura.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="9">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="11">
   <x:si>
     <x:t>factura</x:t>
   </x:si>
@@ -125,6 +125,39 @@
   </x:si>
   <x:si>
     <x:t>VESTIDO LARGO P/DAMA MX1190 MARIA BONITA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01135036</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T010005584</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0001</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T3C1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>VSUAREZ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CT3000000000001</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>03000038</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGUACATE  010075</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -529,7 +562,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B1" s="6" t="s">
-        <x:v>18</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="2">
@@ -537,7 +570,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="B2" s="6" t="s">
-        <x:v>19</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="3">
@@ -545,7 +578,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B3" s="6" t="s">
-        <x:v>20</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="4">
@@ -553,7 +586,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B4" s="6" t="s">
-        <x:v>21</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -561,7 +594,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="B5" s="6" t="s">
-        <x:v>22</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="6">
@@ -569,7 +602,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="B6" s="6" t="s">
-        <x:v>23</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="7">
@@ -577,7 +610,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="B7" s="6" t="s">
-        <x:v>24</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="8">
@@ -585,7 +618,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="B8" s="6">
-        <x:v>36.351</x:v>
+        <x:v>36.5635</x:v>
       </x:c>
     </x:row>
     <x:row r="9">
@@ -598,16 +631,16 @@
       <x:c r="A10" s="4" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="B10" s="3">
-        <x:v>0</x:v>
+      <x:c r="B10" s="3" t="s">
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="11">
       <x:c r="A11" s="4" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="B11" s="3">
-        <x:v>0</x:v>
+      <x:c r="B11" s="3" t="s">
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="12">
@@ -772,7 +805,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{9E17AE92-C25F-4C7B-B325-5A61F6EF2FEC}" mc:Ignorable="x14ac xr xr2 xr3">
-  <x:dimension ref="A1:I6"/>
+  <x:dimension ref="A1:I2"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
       <x:selection activeCell="D6" sqref="D6"/>
@@ -814,84 +847,16 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B2" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="C2">
-        <x:v>2</x:v>
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="C2" t="s">
+        <x:v>44</x:v>
       </x:c>
       <x:c r="D2">
         <x:v>0</x:v>
       </x:c>
       <x:c r="E2" t="s">
-        <x:v>26</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3">
-      <x:c r="A3">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B3" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="C3">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="D3">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E3" t="s">
-        <x:v>28</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4">
-      <x:c r="A4">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="B4" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="C4">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="D4">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="E4" t="s">
-        <x:v>30</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5">
-      <x:c r="A5">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B5" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="C5">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="D5">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E5" t="s">
-        <x:v>32</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6">
-      <x:c r="A6">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B6" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="C6">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="D6">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E6" t="s">
-        <x:v>34</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
diseñando el form autorecuperacion
</commit_message>
<xml_diff>
--- a/COVENTAF/bin/Debug/Auto_Recuperacion_Factura.xlsx
+++ b/COVENTAF/bin/Debug/Auto_Recuperacion_Factura.xlsx
@@ -7,7 +7,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROYECTOS\COVENTAF-DESK\coventaf_desk4.7\COVENTAF\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A837EC7-2618-4055-BCF4-A426F4C4279D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE85184-5AB0-456D-AF33-6269C240B346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1"/>
   </x:bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="11">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
   <x:si>
     <x:t>factura</x:t>
   </x:si>
@@ -46,12 +46,6 @@
     <x:t>Observacion</x:t>
   </x:si>
   <x:si>
-    <x:t>% Descuento General</x:t>
-  </x:si>
-  <x:si>
-    <x:t>% Descuento Autorizado</x:t>
-  </x:si>
-  <x:si>
     <x:t>Linea</x:t>
   </x:si>
   <x:si>
@@ -76,10 +70,25 @@
     <x:t>Descripcion</x:t>
   </x:si>
   <x:si>
-    <x:t>0381125</x:t>
-  </x:si>
-  <x:si>
-    <x:t>T020035586</x:t>
+    <x:t>03000038</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGUACATE  010075</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Descuento_General</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Descuento Autorizado</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0381128</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T010005584</x:t>
   </x:si>
   <x:si>
     <x:t>EXHI</x:t>
@@ -91,73 +100,28 @@
     <x:t>OSCAR</x:t>
   </x:si>
   <x:si>
-    <x:t>CT1000000006681</x:t>
+    <x:t>CT1000000006682</x:t>
   </x:si>
   <x:si>
     <x:t>T01</x:t>
   </x:si>
   <x:si>
-    <x:t>01000517</x:t>
-  </x:si>
-  <x:si>
-    <x:t>VESTIDO LARGO P/DAMA 6814A MARIA BONITA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>01000516</x:t>
-  </x:si>
-  <x:si>
-    <x:t>VESTIDO LARGO P/DAMA 6951 MARIA BONITA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>01000336</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CAMISOLA DEPORT P/DAMA 928989 NIKE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>01000353</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PANTALON JEANS P/DAMA LANE-47-212 U.S. POLO ASSOCIATIO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>01000518</x:t>
-  </x:si>
-  <x:si>
-    <x:t>VESTIDO LARGO P/DAMA MX1190 MARIA BONITA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>01135036</x:t>
-  </x:si>
-  <x:si>
-    <x:t>T010005584</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0001</x:t>
-  </x:si>
-  <x:si>
-    <x:t>T3C1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>VSUAREZ</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CT3000000000001</x:t>
-  </x:si>
-  <x:si>
-    <x:t>T03</x:t>
-  </x:si>
-  <x:si>
     <x:t>0.00</x:t>
   </x:si>
   <x:si>
-    <x:t>03000038</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>AGUACATE  010075</x:t>
+    <x:t>05002299</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PAQUETE DE CALZONES SUPER P/NIÑA 2110006301 ST.JACK</x:t>
+  </x:si>
+  <x:si>
+    <x:t>05001987</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CALCETINES P/NIÑO BLANCO 7-9 WMZ174B/717 REDPOIT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -234,7 +198,7 @@
   <x:cellStyleXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </x:cellStyleXfs>
-  <x:cellXfs count="9">
+  <x:cellXfs count="11">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -244,6 +208,8 @@
     <x:xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <x:xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <x:xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <x:xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,102 +512,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
-  <x:dimension ref="A1:D62"/>
+  <x:dimension ref="A1:K62"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0">
-      <x:selection activeCell="C11" sqref="C11"/>
+      <x:selection activeCell="A2" sqref="A2"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <x:col min="1" max="1" width="15.140625" customWidth="1"/>
+    <x:col min="2" max="2" width="18" customWidth="1"/>
+    <x:col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <x:col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <x:col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <x:col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <x:col min="8" max="8" width="13" customWidth="1"/>
+    <x:col min="9" max="9" width="15" customWidth="1"/>
+    <x:col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
+    <x:col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1">
-      <x:c r="A1" s="5" t="s">
+      <x:c r="A1" s="4" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="6" t="s">
-        <x:v>35</x:v>
+      <x:c r="B1" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C1" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D1" s="4" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E1" s="4" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F1" s="4" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="G1" s="4" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H1" s="4" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I1" s="4" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="J1" s="4" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="K1" s="4" t="s">
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="2">
-      <x:c r="A2" s="5" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B2" s="6" t="s">
-        <x:v>36</x:v>
+      <x:c r="A2" s="9" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B2" s="3" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C2" s="3" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D2" s="3" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E2" s="3" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="F2" s="3" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="G2" s="3" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="H2" s="10">
+        <x:v>36.351</x:v>
+      </x:c>
+      <x:c r="I2" s="3"/>
+      <x:c r="J2" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="K2" s="10" t="s">
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="3">
-      <x:c r="A3" s="5" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B3" s="6" t="s">
-        <x:v>37</x:v>
-      </x:c>
+      <x:c r="A3" s="5"/>
     </x:row>
     <x:row r="4">
-      <x:c r="A4" s="5" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B4" s="6" t="s">
-        <x:v>38</x:v>
-      </x:c>
+      <x:c r="A4" s="5"/>
+      <x:c r="B4" s="4"/>
     </x:row>
     <x:row r="5">
-      <x:c r="A5" s="5" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="B5" s="6" t="s">
-        <x:v>39</x:v>
-      </x:c>
+      <x:c r="A5" s="5"/>
     </x:row>
     <x:row r="6">
-      <x:c r="A6" s="5" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="B6" s="6" t="s">
-        <x:v>40</x:v>
-      </x:c>
+      <x:c r="A6" s="5"/>
     </x:row>
     <x:row r="7">
-      <x:c r="A7" s="5" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="B7" s="6" t="s">
-        <x:v>41</x:v>
-      </x:c>
+      <x:c r="A7" s="5"/>
     </x:row>
     <x:row r="8">
-      <x:c r="A8" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="B8" s="6">
-        <x:v>36.5635</x:v>
-      </x:c>
+      <x:c r="A8" s="5"/>
     </x:row>
     <x:row r="9">
-      <x:c r="A9" s="7" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="B9" s="8"/>
+      <x:c r="A9" s="7"/>
     </x:row>
     <x:row r="10">
-      <x:c r="A10" s="4" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="B10" s="3" t="s">
-        <x:v>42</x:v>
-      </x:c>
+      <x:c r="A10" s="4"/>
     </x:row>
     <x:row r="11">
-      <x:c r="A11" s="4" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B11" s="3" t="s">
-        <x:v>42</x:v>
-      </x:c>
+      <x:c r="A11" s="4"/>
+      <x:c r="B11" s="3"/>
     </x:row>
     <x:row r="12">
       <x:c r="B12" s="3"/>
@@ -664,36 +650,47 @@
       <x:c r="B17" s="3"/>
     </x:row>
     <x:row r="18">
-      <x:c r="B18" s="3"/>
+      <x:c r="A18" s="5"/>
+      <x:c r="B18" s="6"/>
     </x:row>
     <x:row r="19">
-      <x:c r="B19" s="3"/>
+      <x:c r="A19" s="5"/>
+      <x:c r="B19" s="6"/>
     </x:row>
     <x:row r="20">
-      <x:c r="B20" s="3"/>
+      <x:c r="A20" s="5"/>
+      <x:c r="B20" s="6"/>
     </x:row>
     <x:row r="21">
-      <x:c r="B21" s="3"/>
+      <x:c r="A21" s="5"/>
+      <x:c r="B21" s="6"/>
     </x:row>
     <x:row r="22">
-      <x:c r="B22" s="3"/>
+      <x:c r="A22" s="5"/>
+      <x:c r="B22" s="6"/>
     </x:row>
     <x:row r="23">
-      <x:c r="B23" s="3"/>
+      <x:c r="A23" s="5"/>
+      <x:c r="B23" s="6"/>
     </x:row>
     <x:row r="24">
-      <x:c r="B24" s="3"/>
+      <x:c r="A24" s="5"/>
+      <x:c r="B24" s="6"/>
     </x:row>
     <x:row r="25">
-      <x:c r="B25" s="3"/>
+      <x:c r="A25" s="5"/>
+      <x:c r="B25" s="6"/>
     </x:row>
     <x:row r="26">
-      <x:c r="B26" s="3"/>
+      <x:c r="A26" s="7"/>
+      <x:c r="B26" s="8"/>
     </x:row>
     <x:row r="27">
+      <x:c r="A27" s="4"/>
       <x:c r="B27" s="3"/>
     </x:row>
     <x:row r="28">
+      <x:c r="A28" s="4"/>
       <x:c r="B28" s="3"/>
     </x:row>
     <x:row r="29">
@@ -805,10 +802,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{9E17AE92-C25F-4C7B-B325-5A61F6EF2FEC}" mc:Ignorable="x14ac xr xr2 xr3">
-  <x:dimension ref="A1:I2"/>
+  <x:dimension ref="A1:I3"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="D6" sqref="D6"/>
+      <x:selection activeCell="A2" sqref="A2"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -820,7 +817,7 @@
   <x:sheetData>
     <x:row r="1">
       <x:c r="A1" s="4" t="s">
-        <x:v>10</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B1" s="4" t="s">
         <x:v>1</x:v>
@@ -832,13 +829,13 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="E1" s="4" t="s">
-        <x:v>17</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="F1" s="4" t="s">
         <x:v>3</x:v>
       </x:c>
       <x:c r="G1" s="4" t="s">
-        <x:v>11</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="I1" s="4"/>
     </x:row>
@@ -847,16 +844,33 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B2" t="s">
-        <x:v>43</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C2" t="s">
-        <x:v>44</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="D2">
         <x:v>0</x:v>
       </x:c>
       <x:c r="E2" t="s">
-        <x:v>45</x:v>
+        <x:v>30</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3">
+      <x:c r="A3">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B3" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="C3" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="D3">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E3" t="s">
+        <x:v>32</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
desarrollando punto de venta 26-09-2023
</commit_message>
<xml_diff>
--- a/COVENTAF/bin/Debug/Auto_Recuperacion_Factura.xlsx
+++ b/COVENTAF/bin/Debug/Auto_Recuperacion_Factura.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="11">
   <x:si>
     <x:t>factura</x:t>
   </x:si>
@@ -122,6 +122,282 @@
   </x:si>
   <x:si>
     <x:t>2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01135059</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COC0018</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0001</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T3C5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AYAEL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CT3000000000019</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01000019</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ARROZ PAELLA VIGO 19OZ 012670 S/M 013052</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01000035</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ARROZ FAISAN 96/4 QUINTAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T040000256</x:t>
+  </x:si>
+  <x:si>
+    <x:t>04000217</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TITILES CONG TIP TOP 503054</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01135064</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CT3000000000022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08000045</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9PACK CERVEZA VICTORIA FROST LATA 010040</x:t>
+  </x:si>
+  <x:si>
+    <x:t>03000017</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LIMON S/SEMILLA DOCENA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01000026</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ARROZ 96/04 2KG/11 FAISAN 051152</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>60</x:t>
+  </x:si>
+  <x:si>
+    <x:t>120</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01135065</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01135067</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01135068</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01000028</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ARROZ 96/04 25LBS FAISAN 010030 051190</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01135025</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T3C1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SCAJERO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CT3000000000006</x:t>
+  </x:si>
+  <x:si>
+    <x:t>04000078</x:t>
+  </x:si>
+  <x:si>
+    <x:t>POLLO ENTERO 5-6 LB TIP-TOP 030001</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T010000240</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11.14</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22.28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33.42</x:t>
+  </x:si>
+  <x:si>
+    <x:t>44.56</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25.30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01135080</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T010007963</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T3C11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>VSUAREZ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CT3000000000025</x:t>
+  </x:si>
+  <x:si>
+    <x:t>03000087</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.58</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ESPINACA LB 010142</x:t>
+  </x:si>
+  <x:si>
+    <x:t>03000054</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PLATANO UND 010095</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01135083</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MJIRON</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CT3000000000012</x:t>
+  </x:si>
+  <x:si>
+    <x:t>02000870</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SAZONADOR DE POLLO BOLSA 13GR (12) 019026 MAYA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01000008</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ARROZ 80/20 GRANEL 010067</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T020002654</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01000052</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ARROZ BOLSA 80/20 400GRX25 120208 IMPERIO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T020006611</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T020037352</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T010008371</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01000027</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ARROZ 96/04 400G/25 FAISAN 051176</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01135084</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T020011219</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T020044101</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T020067460</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01000483</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LECHE CHOCOLATE BOLSA 400ML 211723 ESKIMO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T020008377</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T040000216</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T020035684</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01000030</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ARROZ 96/04 10LBX5 FAISAN 051275</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01000020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ARROZ BASMATI 2LB/6 030219 VIGO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T050010798</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T3C10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SARGUELLO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CT3000000000026</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12000013</x:t>
+  </x:si>
+  <x:si>
+    <x:t>POSTA DE PIERNA S/R S/M</x:t>
+  </x:si>
+  <x:si>
+    <x:t>03000042</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BANANO MADURO UND</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T010005360</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -520,16 +796,15 @@
   </x:sheetViews>
   <x:sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="15.140625" customWidth="1"/>
-    <x:col min="2" max="2" width="18" customWidth="1"/>
-    <x:col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <x:col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <x:col min="1" max="1" width="15" customWidth="1"/>
+    <x:col min="2" max="3" width="18" customWidth="1"/>
+    <x:col min="4" max="4" width="17" customWidth="1"/>
     <x:col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <x:col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <x:col min="7" max="7" width="12" customWidth="1"/>
     <x:col min="8" max="8" width="13" customWidth="1"/>
     <x:col min="9" max="9" width="15" customWidth="1"/>
     <x:col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
-    <x:col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
+    <x:col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1">
@@ -569,28 +844,28 @@
     </x:row>
     <x:row r="2">
       <x:c r="A2" s="9" t="s">
-        <x:v>21</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="B2" s="3" t="s">
-        <x:v>22</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="C2" s="3" t="s">
-        <x:v>23</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="D2" s="3" t="s">
-        <x:v>24</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="E2" s="3" t="s">
-        <x:v>25</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="F2" s="3" t="s">
-        <x:v>26</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="G2" s="3" t="s">
-        <x:v>27</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="H2" s="10">
-        <x:v>36.351</x:v>
+        <x:v>36.5635</x:v>
       </x:c>
       <x:c r="I2" s="3"/>
       <x:c r="J2" s="10" t="s">
@@ -802,7 +1077,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{9E17AE92-C25F-4C7B-B325-5A61F6EF2FEC}" mc:Ignorable="x14ac xr xr2 xr3">
-  <x:dimension ref="A1:I3"/>
+  <x:dimension ref="A1:I2"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
       <x:selection activeCell="A2" sqref="A2"/>
@@ -844,7 +1119,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B2" t="s">
-        <x:v>29</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C2" t="s">
         <x:v>17</x:v>
@@ -853,24 +1128,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="E2" t="s">
-        <x:v>30</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3">
-      <x:c r="A3">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B3" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="C3" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="D3">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E3" t="s">
-        <x:v>32</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>